<commit_message>
Added I2C pins and hi-pro compatible plates
</commit_message>
<xml_diff>
--- a/bom/shark_LCSC.xlsx
+++ b/bom/shark_LCSC.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="70">
   <si>
     <t>Description</t>
   </si>
@@ -193,7 +193,7 @@
     <t>C114585</t>
   </si>
   <si>
-    <t>RL1-RL (360 Ohm 1206)</t>
+    <t>RL1-RL51 (360 Ohm 1206)</t>
   </si>
   <si>
     <t>C25376</t>
@@ -209,6 +209,18 @@
   </si>
   <si>
     <t>C370970</t>
+  </si>
+  <si>
+    <t>I2C JST connector</t>
+  </si>
+  <si>
+    <t>C265374</t>
+  </si>
+  <si>
+    <t>I2C JST header</t>
+  </si>
+  <si>
+    <t>C265032</t>
   </si>
 </sst>
 </file>
@@ -242,18 +254,19 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -287,14 +300,13 @@
     <col customWidth="1" min="5" max="6" width="22.29"/>
     <col customWidth="1" min="7" max="7" width="5.86"/>
     <col customWidth="1" min="8" max="8" width="25.86"/>
-    <col customWidth="1" min="9" max="25" width="8.71"/>
   </cols>
   <sheetData>
     <row r="1" ht="14.25" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
@@ -883,14 +895,14 @@
       </c>
     </row>
     <row r="24" ht="14.25" customHeight="1">
-      <c r="A24" t="s">
+      <c r="A24" s="2" t="s">
         <v>60</v>
       </c>
       <c r="B24" t="s">
         <v>61</v>
       </c>
-      <c r="C24">
-        <v>50.0</v>
+      <c r="C24" s="2">
+        <v>51.0</v>
       </c>
       <c r="D24">
         <v>0.0023</v>
@@ -942,6 +954,28 @@
         <v>65</v>
       </c>
       <c r="C26" s="3">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="27" ht="15.75" customHeight="1">
+      <c r="A27" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="C27" s="2">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="28" ht="15.75" customHeight="1">
+      <c r="A28" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="C28" s="2">
         <v>1.0</v>
       </c>
     </row>

</xml_diff>